<commit_message>
Updated files for Veils
</commit_message>
<xml_diff>
--- a/veils/hardware_design/Veils.xlsx
+++ b/veils/hardware_design/Veils.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="3620" windowWidth="32900" windowHeight="22500" tabRatio="484"/>
+    <workbookView xWindow="16320" yWindow="3660" windowWidth="32900" windowHeight="22500" tabRatio="484"/>
   </bookViews>
   <sheets>
-    <sheet name="Veils v4.0a" sheetId="5" r:id="rId1"/>
+    <sheet name="Veils v11.0" sheetId="7" r:id="rId1"/>
+    <sheet name="Veils v4.0a" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="218">
   <si>
     <t>Index</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Ref. Mouser</t>
   </si>
   <si>
-    <t>S. MI</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
@@ -120,9 +118,6 @@
     <t>Vertical jack connector</t>
   </si>
   <si>
-    <t>PJ-301-M-12</t>
-  </si>
-  <si>
     <t>PTH parts, bottom side</t>
   </si>
   <si>
@@ -421,16 +416,275 @@
   </si>
   <si>
     <t>https://www.thonk.co.uk/shop/alpha-9mm-pots/</t>
+  </si>
+  <si>
+    <t>Veils, v11.0</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>2.0k</t>
+  </si>
+  <si>
+    <t>667-ERJ-2RKF2001X</t>
+  </si>
+  <si>
+    <t>R5, R10, R11, R12, R13, R61, R62, R63, R64, R78, R79, R80, R81</t>
+  </si>
+  <si>
+    <t>24.9k</t>
+  </si>
+  <si>
+    <t>667-ERJ-2RKF2492X</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9</t>
+  </si>
+  <si>
+    <t>R14, R15, R16, R17</t>
+  </si>
+  <si>
+    <t>120k</t>
+  </si>
+  <si>
+    <t>667-ERJ-2RKF1203X</t>
+  </si>
+  <si>
+    <t>R18, R19, R20, R21</t>
+  </si>
+  <si>
+    <t>R22, R23, R56</t>
+  </si>
+  <si>
+    <t>R24, R25, R26, R27, R28, R29, R30, R53, R54, R55, R57, R58, R59, R60</t>
+  </si>
+  <si>
+    <t>R31, R32, R35, R36, R37, R38, R45, R46, R47, R48, R51, R52</t>
+  </si>
+  <si>
+    <t>R33, R34</t>
+  </si>
+  <si>
+    <t>680k</t>
+  </si>
+  <si>
+    <t>667-ERJ-2RKF6803X</t>
+  </si>
+  <si>
+    <t>R39, R40, R41, R42, R43, R44, R49, R50, R69</t>
+  </si>
+  <si>
+    <t>R65, R66, R67, R68, R70, R71, R72, R73, R74, R75, R76, R77, R82, R83, R84, R85, R86, R87, R88, R89</t>
+  </si>
+  <si>
+    <t>603-RC0402FR-071ML</t>
+  </si>
+  <si>
+    <t>R90, R91, R92, R93</t>
+  </si>
+  <si>
+    <t>R94, R95, R96, R97</t>
+  </si>
+  <si>
+    <t>667-ERJ-PA3J511V</t>
+  </si>
+  <si>
+    <t>&gt;= 1k ohm, 300mA</t>
+  </si>
+  <si>
+    <t>Würth Electronics 742792664</t>
+  </si>
+  <si>
+    <t>C1, C42, C43, C44, C45, C46</t>
+  </si>
+  <si>
+    <t>&gt;= 35V, X5R</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>81-GRM188R6YA225MA2D</t>
+  </si>
+  <si>
+    <t>Murata GRM188R6YA225MA12D</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C10, C11, C12, C13, C18, C19, C26, C29, C34, C37, C38, C39, C47, C48, C49, C50</t>
+  </si>
+  <si>
+    <t>&gt;= 25V, X5R</t>
+  </si>
+  <si>
+    <t>710-885012105018</t>
+  </si>
+  <si>
+    <t>Würth 885012105018</t>
+  </si>
+  <si>
+    <t>C6, C7, C35, C36</t>
+  </si>
+  <si>
+    <t>81-GRM31CC81E226KE1L</t>
+  </si>
+  <si>
+    <t>Murata GRM31CC81E226KE11L</t>
+  </si>
+  <si>
+    <t>C8, C9, C14, C15, C16, C17, C30, C31, C32, C33, C40, C41</t>
+  </si>
+  <si>
+    <t>&gt;= 25V, C0G, &lt;= 5%</t>
+  </si>
+  <si>
+    <t>81-GCM1555C1H101FA6D</t>
+  </si>
+  <si>
+    <t>Murata GCM1555C1H101FA16D</t>
+  </si>
+  <si>
+    <t>C20, C21, C22, C23, C24, C25, C27, C28</t>
+  </si>
+  <si>
+    <t>810-CGJ2B2C0G1H561J</t>
+  </si>
+  <si>
+    <t>TDK CGJ2B2C0G1H561J050BA</t>
+  </si>
+  <si>
+    <t>D3, D4, D5, D6</t>
+  </si>
+  <si>
+    <t>1N4148 silicon diode</t>
+  </si>
+  <si>
+    <t>SOD523</t>
+  </si>
+  <si>
+    <t>512-1N4148WT</t>
+  </si>
+  <si>
+    <t>Fairchild Semi 1N4148WT</t>
+  </si>
+  <si>
+    <t>&gt; 0.1A</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>C Grade, 0.5%</t>
+  </si>
+  <si>
+    <t>IC2, IC3, IC6, IC7</t>
+  </si>
+  <si>
+    <t>OPA1679 Quad op-amp</t>
+  </si>
+  <si>
+    <t>595-OPA1679IPWR</t>
+  </si>
+  <si>
+    <t>Texas instruments OPA1679IPWR</t>
+  </si>
+  <si>
+    <t>IC4, IC5</t>
+  </si>
+  <si>
+    <t>V2164 Quad VCA</t>
+  </si>
+  <si>
+    <t>IC9, IC10</t>
+  </si>
+  <si>
+    <t>LM324 Quad op-amp</t>
+  </si>
+  <si>
+    <t>595-LM324PWR</t>
+  </si>
+  <si>
+    <t>Texas Instruments LM324PWR</t>
+  </si>
+  <si>
+    <t>SMT parts (hand-soldered)</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>2x5 Header, 2.54 pitch</t>
+  </si>
+  <si>
+    <t>571-5-146135-4</t>
+  </si>
+  <si>
+    <t>LED, Red/Green, 2 terminals</t>
+  </si>
+  <si>
+    <t>2 terminals</t>
+  </si>
+  <si>
+    <t>749-3BC-F</t>
+  </si>
+  <si>
+    <t>Bivar 3BC-F</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>LED holder, 8.89mm</t>
+  </si>
+  <si>
+    <t>749-ELM-4-350</t>
+  </si>
+  <si>
+    <t>Bivar ELM 4-350</t>
+  </si>
+  <si>
+    <t>R98, R99, R100, R101</t>
+  </si>
+  <si>
+    <t>20k linear slide pot, green LED</t>
+  </si>
+  <si>
+    <t>R102, R103, R104, R105</t>
+  </si>
+  <si>
+    <t>50k linear pot, 25mm shaft with marker</t>
+  </si>
+  <si>
+    <t>R106, R107, R108, R109</t>
+  </si>
+  <si>
+    <t>49.0 x 106.7, 4 layers</t>
+  </si>
+  <si>
+    <t>V2164M</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/thonkiconn/</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/alpha-sliders/</t>
+  </si>
+  <si>
+    <t>652-PTL20-15G1-203B2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.###############"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -499,6 +753,30 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -526,7 +804,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -552,8 +830,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="355">
+  <cellStyleXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -909,8 +1205,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -982,6 +1283,7 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -991,9 +1293,148 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="355" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="355" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="355" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="355" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="355" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="355" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="355" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="355" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="355" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="355" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="355" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="355" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="355">
+  <cellStyles count="358">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1171,6 +1612,7 @@
     <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1348,7 +1790,9 @@
     <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="355"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1677,10 +2121,969 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.83203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="66" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="77" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="32" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="34" customHeight="1">
+      <c r="A1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="12" thickBot="1">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12" customHeight="1">
+      <c r="A3" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:8" s="44" customFormat="1">
+      <c r="A4" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="41">
+        <v>4</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="42" t="str">
+        <f>"&lt;=1%, 100mW"</f>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="43" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="45"/>
+    </row>
+    <row r="5" spans="1:8" s="44" customFormat="1">
+      <c r="A5" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="41">
+        <v>13</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="42" t="str">
+        <f t="shared" ref="D5:D15" si="0">"&lt;=1%, 100mW"</f>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="43" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="1:8" s="44" customFormat="1">
+      <c r="A6" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="41">
+        <v>4</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="43" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:8" s="44" customFormat="1">
+      <c r="A7" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="41">
+        <v>4</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="43" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:8" s="44" customFormat="1">
+      <c r="A8" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="41">
+        <v>4</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="42" t="str">
+        <f>"&lt;=5%, 100mW"</f>
+        <v>&lt;=5%, 100mW</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="43" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="45"/>
+    </row>
+    <row r="9" spans="1:8" s="44" customFormat="1">
+      <c r="A9" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="41">
+        <v>3</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="43" t="str">
+        <f t="shared" ref="F9:F15" si="1">"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="45"/>
+    </row>
+    <row r="10" spans="1:8" s="44" customFormat="1" ht="22">
+      <c r="A10" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="41">
+        <v>14</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" s="44" customFormat="1">
+      <c r="A11" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="41">
+        <v>12</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="45"/>
+    </row>
+    <row r="12" spans="1:8" s="44" customFormat="1">
+      <c r="A12" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="41">
+        <v>2</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" s="45"/>
+    </row>
+    <row r="13" spans="1:8" s="44" customFormat="1">
+      <c r="A13" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="41">
+        <v>9</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E13" s="40">
+        <v>510</v>
+      </c>
+      <c r="F13" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="1:8" s="44" customFormat="1" ht="22">
+      <c r="A14" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="41">
+        <v>20</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="45"/>
+    </row>
+    <row r="15" spans="1:8" s="44" customFormat="1">
+      <c r="A15" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="41">
+        <v>4</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;=1%, 100mW</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>0402</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="45"/>
+    </row>
+    <row r="16" spans="1:8" s="44" customFormat="1">
+      <c r="A16" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="41">
+        <v>4</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="42" t="str">
+        <f>"&lt;=5%, 250mW"</f>
+        <v>&lt;=5%, 250mW</v>
+      </c>
+      <c r="E16" s="40">
+        <v>510</v>
+      </c>
+      <c r="F16" s="43" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="1:21" s="44" customFormat="1">
+      <c r="A17" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="42">
+        <v>2</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="48" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="44" customFormat="1">
+      <c r="A18" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="42">
+        <v>6</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" s="50" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="44" customFormat="1" ht="22">
+      <c r="A19" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="42">
+        <v>20</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="52" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="44" customFormat="1">
+      <c r="A20" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="41">
+        <v>4</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="43">
+        <v>1206</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="44" customFormat="1">
+      <c r="A21" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="42">
+        <v>12</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="52" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="44" customFormat="1">
+      <c r="A22" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="42">
+        <v>8</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="52" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="44" customFormat="1">
+      <c r="A23" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="42">
+        <v>2</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="44" customFormat="1">
+      <c r="A24" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="47">
+        <v>4</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="44" customFormat="1">
+      <c r="A25" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="53">
+        <v>1</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25" s="54">
+        <v>1206</v>
+      </c>
+      <c r="G25" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="55"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53"/>
+      <c r="T25" s="53"/>
+      <c r="U25" s="53"/>
+    </row>
+    <row r="26" spans="1:21" s="44" customFormat="1">
+      <c r="A26" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="42">
+        <v>1</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="44" customFormat="1">
+      <c r="A27" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="42">
+        <v>4</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="55"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="44" customFormat="1">
+      <c r="A28" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="42">
+        <v>2</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="44" customFormat="1">
+      <c r="A29" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="42">
+        <v>1</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="44" customFormat="1">
+      <c r="A30" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="42">
+        <v>2</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="12" customHeight="1">
+      <c r="A31" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+    </row>
+    <row r="32" spans="1:21" s="44" customFormat="1">
+      <c r="A32" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" s="44">
+        <v>1</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="H32" s="55"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="61"/>
+    </row>
+    <row r="34" spans="1:8" s="44" customFormat="1">
+      <c r="A34" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="44">
+        <v>12</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="44" customFormat="1">
+      <c r="A35" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="44">
+        <v>4</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="G35" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="H35" s="67" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="44" customFormat="1">
+      <c r="A36" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" s="42">
+        <v>4</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="44" customFormat="1">
+      <c r="A37" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" s="44">
+        <v>4</v>
+      </c>
+      <c r="C37" s="68" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="H37" s="71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="44" customFormat="1">
+      <c r="A38" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="44">
+        <v>4</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="44" customFormat="1">
+      <c r="A39" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="44">
+        <v>4</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="47"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="72"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A31:G31"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1692,26 +3095,24 @@
     <col min="5" max="5" width="6" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="39.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="29" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-    </row>
-    <row r="2" spans="1:22" ht="16" customHeight="1" thickBot="1">
+    <row r="1" spans="1:21" ht="29" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:21" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1736,9 +3137,7 @@
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1751,21 +3150,20 @@
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-    </row>
-    <row r="3" spans="1:22" s="15" customFormat="1" ht="12.75" customHeight="1" thickTop="1">
-      <c r="A3" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+    </row>
+    <row r="3" spans="1:21" s="15" customFormat="1" ht="12.75" customHeight="1" thickTop="1">
+      <c r="A3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
@@ -1777,17 +3175,16 @@
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-    </row>
-    <row r="4" spans="1:22">
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="23">
         <v>16</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="7">
         <v>510</v>
@@ -1797,8 +3194,9 @@
         <v>0402</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>67</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -1810,28 +3208,28 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-    </row>
-    <row r="5" spans="1:22">
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" s="23">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>87</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -1843,28 +3241,28 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-    </row>
-    <row r="6" spans="1:22">
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B6" s="23">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>79</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1876,29 +3274,29 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-    </row>
-    <row r="7" spans="1:22">
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" s="23">
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -1910,29 +3308,29 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-    </row>
-    <row r="8" spans="1:22">
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1944,28 +3342,28 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-    </row>
-    <row r="9" spans="1:22">
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="23">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>73</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1977,28 +3375,28 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-    </row>
-    <row r="10" spans="1:22">
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="23">
         <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="F10" s="7" t="str">
         <f>"0402"</f>
         <v>0402</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>70</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -2010,28 +3408,28 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-    </row>
-    <row r="11" spans="1:22">
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="23">
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F11" s="7" t="str">
         <f t="shared" ref="F11:F18" si="1">"0402"</f>
         <v>0402</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>130</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -2043,29 +3441,29 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-    </row>
-    <row r="12" spans="1:22">
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="23">
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>71</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -2077,29 +3475,29 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-    </row>
-    <row r="13" spans="1:22">
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" s="23">
         <v>4</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -2111,31 +3509,31 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-    </row>
-    <row r="14" spans="1:22">
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="23">
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>117</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -2147,34 +3545,34 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-    </row>
-    <row r="15" spans="1:22">
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15" s="23">
         <v>4</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F15" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -2186,34 +3584,34 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-    </row>
-    <row r="16" spans="1:22">
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="23">
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>89</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -2225,34 +3623,34 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-    </row>
-    <row r="17" spans="1:22">
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="23">
         <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -2264,34 +3662,34 @@
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-    </row>
-    <row r="18" spans="1:22">
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="23">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F18" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -2303,33 +3701,33 @@
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-    </row>
-    <row r="19" spans="1:22" ht="22">
+    </row>
+    <row r="19" spans="1:21" ht="22">
       <c r="A19" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" s="7">
         <v>4</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -2341,27 +3739,27 @@
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-    </row>
-    <row r="20" spans="1:22">
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="23">
         <v>2</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="H20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -2373,33 +3771,33 @@
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-    </row>
-    <row r="21" spans="1:22">
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="7">
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F21" s="7">
         <v>1206</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -2411,21 +3809,21 @@
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-    </row>
-    <row r="22" spans="1:22">
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" s="7">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -2437,30 +3835,29 @@
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="1:22">
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B23" s="7">
         <v>4</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17" t="s">
-        <v>57</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -2472,30 +3869,29 @@
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-    </row>
-    <row r="24" spans="1:22">
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="7">
         <v>2</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="19"/>
       <c r="F24" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -2507,34 +3903,33 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-    </row>
-    <row r="25" spans="1:22">
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="7">
         <v>1</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="26">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17" t="s">
-        <v>122</v>
-      </c>
+      <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -2546,33 +3941,33 @@
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-    </row>
-    <row r="26" spans="1:22">
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B26" s="7">
         <v>1</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="26">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -2584,20 +3979,19 @@
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-    </row>
-    <row r="27" spans="1:22">
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" s="23">
         <v>2</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="20" t="str">
@@ -2605,12 +3999,12 @@
         <v>0603</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -2622,23 +4016,22 @@
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-    </row>
-    <row r="28" spans="1:22" s="15" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="29" t="s">
+    </row>
+    <row r="28" spans="1:21" s="15" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A28" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
@@ -2650,21 +4043,21 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
       <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-    </row>
-    <row r="29" spans="1:22">
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="7">
         <v>12</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -2676,24 +4069,24 @@
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-    </row>
-    <row r="30" spans="1:22">
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="7">
         <v>4</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -2705,9 +4098,8 @@
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
       <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-    </row>
-    <row r="31" spans="1:22">
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="22" t="str">
         <f>"- LED1, LED2, LED3, LED4"</f>
         <v>- LED1, LED2, LED3, LED4</v>
@@ -2716,14 +4108,15 @@
         <v>4</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>93</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -2735,26 +4128,25 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-    </row>
-    <row r="32" spans="1:22">
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B32" s="23">
         <v>4</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="30" t="s">
-        <v>132</v>
-      </c>
+      <c r="H32" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="7"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
@@ -2766,21 +4158,21 @@
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-    </row>
-    <row r="33" spans="1:22">
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B33" s="23">
         <v>4</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -2792,11 +4184,10 @@
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-    </row>
-    <row r="34" spans="1:22" s="15" customFormat="1">
+    </row>
+    <row r="34" spans="1:21" s="15" customFormat="1">
       <c r="A34" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="9"/>
@@ -2806,7 +4197,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="J34" s="16"/>
       <c r="K34" s="16"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
@@ -2818,26 +4209,25 @@
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-    </row>
-    <row r="35" spans="1:22">
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
+      <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
@@ -2849,27 +4239,26 @@
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="7"/>
-    </row>
-    <row r="36" spans="1:22" s="12" customFormat="1">
+    </row>
+    <row r="36" spans="1:21" s="12" customFormat="1">
       <c r="A36" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:21">
       <c r="C37" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A28:G28"/>
   </mergeCells>

</xml_diff>